<commit_message>
add 'AddEvent' to calendar
</commit_message>
<xml_diff>
--- a/documents/module.xlsx
+++ b/documents/module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\Comraids\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30479225-602F-4C31-BA1C-3DE0E0DAECA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5345FA16-B126-4074-B46C-949A530ED2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="3510" windowWidth="28800" windowHeight="15435" xr2:uid="{2F59410A-04CD-4807-91D3-54AADDE936A0}"/>
+    <workbookView xWindow="5505" yWindow="3285" windowWidth="28800" windowHeight="15435" xr2:uid="{2F59410A-04CD-4807-91D3-54AADDE936A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>calendar</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>region</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>달력 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>달력 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멤버 관리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -481,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2CCA24-2C30-46E6-9765-E0DFFC7D1BDD}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -574,6 +586,21 @@
         <v>17</v>
       </c>
     </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Backend: adding calendar apis
</commit_message>
<xml_diff>
--- a/documents/module.xlsx
+++ b/documents/module.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\Comraids\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5345FA16-B126-4074-B46C-949A530ED2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1267B85A-6FDE-46F8-B5B7-B4F823607F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="3285" windowWidth="28800" windowHeight="15435" xr2:uid="{2F59410A-04CD-4807-91D3-54AADDE936A0}"/>
+    <workbookView xWindow="840" yWindow="1575" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{2F59410A-04CD-4807-91D3-54AADDE936A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -194,6 +195,1136 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="직사각형 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F887AB3A-7562-4B3E-B75F-473CFBDD7FFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="962025" y="600076"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>주소 입력</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="순서도: 판단 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C9129AB-FC3C-4F45-AE39-B32978635777}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="647700" y="1819275"/>
+          <a:ext cx="2190750" cy="1247775"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>JWT Cookie?</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="직사각형 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF0565DF-1038-400E-BD8B-9E1205D90E93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3733800" y="2124076"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>자동 로그인</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="직사각형 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{547F2368-DC42-4580-9CBB-8CE69B9BE5C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1009650" y="3657601"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>로그인 화면</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="직사각형 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{706CABB1-6D21-45D8-A409-B7AE89C0C1ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6276975" y="2105026"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>메뉴</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>달력 정보 표시</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="직사각형 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6799CF6B-1C41-4202-B413-1195E9818BCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6076950" y="3038476"/>
+          <a:ext cx="1885950" cy="1247774"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>로컬 스토리지에 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>selectedCalendar(ID) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>참조</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>페이지 로딩 완료 시</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>그 달력이 선택되게</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="직사각형 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA2C8D26-A6E4-48B0-9578-4C1311FE5E91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12449175" y="1066801"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>Local</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t> Storage</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="직사각형 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7FD1E66-66BD-463D-8D85-85042EEFEE09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12449175" y="1962151"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>Region</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="직사각형 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15FB35A3-50B4-4A37-A50F-FE80EA3561A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12449175" y="2838451"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>selected</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t> calendar</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="직사각형 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A6AA48D-928A-4D96-8786-C87EDCEC656D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14268450" y="1066801"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>Cookie</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="직사각형 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6A85E00-2B04-49F7-9C88-1A89493CC0E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14268450" y="1962151"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>JWT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t> Token</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="직사각형 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6F4414C-891A-476A-ACD2-0D5B508801C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14268450" y="2838451"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>CSRF</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t> Token</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="직사각형 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ED99C41-3001-463A-87AD-C40B994D14E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12211050" y="657225"/>
+          <a:ext cx="3810000" cy="3476625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1171575" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5F595CB-BA27-4501-ABD6-3883E8167465}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13515975" y="285750"/>
+          <a:ext cx="1171575" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600"/>
+            <a:t>In Browser</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1600"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647699</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="직사각형 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0A5ECD6-0116-4354-9A03-DA5E9AC52126}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3514724" y="3152775"/>
+          <a:ext cx="1933575" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>JWT Cookie </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>정보로</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>DB</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>에서 유저 정보 습득</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>Context</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>에 저장</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>프론트</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t>서버 최초 접속 시</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t>, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t>새 페이지</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100" baseline="0"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="직사각형 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0B01A23-9AE9-49DB-843F-7E7E9D8CB2CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8582025" y="2143126"/>
+          <a:ext cx="1504950" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>메뉴</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1100"/>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            <a:t>달력 정보 표시</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -481,7 +1612,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+      <a:lstStyle>
+        <a:defPPr algn="ctr">
+          <a:defRPr sz="1100"/>
+        </a:defPPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -495,7 +1650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2CCA24-2C30-46E6-9765-E0DFFC7D1BDD}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -606,4 +1761,20 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C000B47-8E53-40F5-B259-A4892F64C7D6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>